<commit_message>
Fixed issues in alloys and periodic table
</commit_message>
<xml_diff>
--- a/scripts/Periodic-Table.xlsx
+++ b/scripts/Periodic-Table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="231">
   <si>
     <t xml:space="preserve">Atomic number</t>
   </si>
@@ -688,7 +688,7 @@
     <t xml:space="preserve">Lr</t>
   </si>
   <si>
-    <t xml:space="preserve">Rare earth</t>
+    <t xml:space="preserve">Rare Earths</t>
   </si>
   <si>
     <t xml:space="preserve">RE</t>
@@ -700,31 +700,19 @@
     <t xml:space="preserve">Lanthanides</t>
   </si>
   <si>
-    <t xml:space="preserve">Lnd</t>
+    <t xml:space="preserve">Lad</t>
   </si>
   <si>
     <t xml:space="preserve">Usually means lanthanum</t>
   </si>
   <si>
-    <t xml:space="preserve">Didymium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Usually includes praseodymium and neodymium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mischmetal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Usually includes cerium, lanthanum, and neodyminum</t>
-  </si>
-  <si>
     <t xml:space="preserve">Actinides</t>
   </si>
   <si>
     <t xml:space="preserve">Acd</t>
   </si>
   <si>
-    <t xml:space="preserve">Usually includes Uranium</t>
+    <t xml:space="preserve">Usually means uranium</t>
   </si>
 </sst>
 </file>
@@ -758,18 +746,12 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -811,7 +793,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -832,10 +814,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A104" activeCellId="0" sqref="A104"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E102" activeCellId="0" sqref="E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2061,7 +2043,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="n">
         <v>105</v>
       </c>
@@ -2082,35 +2064,15 @@
       <c r="B107" s="0" t="s">
         <v>228</v>
       </c>
+      <c r="C107" s="0" t="s">
+        <v>229</v>
+      </c>
       <c r="E107" s="0" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0" t="n">
-        <v>107</v>
-      </c>
-      <c r="B108" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="E108" s="0" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="n">
-        <v>108</v>
-      </c>
-      <c r="B109" s="0" t="s">
-        <v>232</v>
-      </c>
-      <c r="C109" s="0" t="s">
-        <v>233</v>
-      </c>
-      <c r="E109" s="0" t="s">
-        <v>234</v>
-      </c>
-    </row>
+    </row>
+    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>